<commit_message>
Assignment 2 - Task 3 - Week 10 - Answer
1. Implement methods for draw snake and prey.
2. Paint Components - snake and prey
3. Layout Managers
4. Load Snake game when authentication successful.
5. Update product backlog
</commit_message>
<xml_diff>
--- a/local snake game/Product-backlog-AH-23594256.xlsx
+++ b/local snake game/Product-backlog-AH-23594256.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\Desktop\github\PROG5001A2\local snake game\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4BAC0B5-2FCD-49F2-AD02-6E58E8444590}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{49C32462-D2B8-4175-AE19-832EFB3F644D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="2" r:id="rId1"/>
     <sheet name="Snake-game" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Week 9</t>
   </si>
@@ -172,16 +166,25 @@
     <t>3.1.3</t>
   </si>
   <si>
-    <t>Snake</t>
-  </si>
-  <si>
     <t>locate an apple in game board in random location</t>
+  </si>
+  <si>
+    <t>Load Images to GUI</t>
+  </si>
+  <si>
+    <t>Test the gameboard</t>
+  </si>
+  <si>
+    <t>GUI layoutmanager</t>
+  </si>
+  <si>
+    <t>3.1.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,7 +410,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -459,7 +462,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -653,17 +656,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F2A6E6-5A3B-4CAD-BC9F-023E52339F74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -808,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
@@ -871,11 +874,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDA2708-75B5-4180-9C4B-08F40A18D95A}">
-  <dimension ref="A1:L27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1095,7 @@
         <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1101,9 +1104,13 @@
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="B15" s="6"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1192,7 +1199,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="14">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1207,16 +1214,27 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="11">
+        <v>4.2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E28" s="8">
         <v>4</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F28" s="14">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assignment 2 - Task 5 - Week 12 - Answer
1. Game logic Algorithm
 *snake grow
 *check snake collide with board or
  itself.
2. Start and Pause
3. Update Backlog
</commit_message>
<xml_diff>
--- a/local snake game/Product-backlog-AH-23594256.xlsx
+++ b/local snake game/Product-backlog-AH-23594256.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Week 9</t>
   </si>
@@ -188,6 +188,24 @@
   </si>
   <si>
     <t>Test snake and prey</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>game logic algorithm</t>
+  </si>
+  <si>
+    <t>start and pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test snake graw </t>
+  </si>
+  <si>
+    <t>Test start and pause</t>
   </si>
 </sst>
 </file>
@@ -275,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -353,12 +371,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,40 +713,40 @@
       <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -884,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,8 +1100,12 @@
         <v>22</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="38">
+        <v>0.98</v>
+      </c>
+      <c r="I12" s="38">
+        <v>1</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
     </row>
@@ -1092,6 +1116,9 @@
       <c r="B13" s="6"/>
       <c r="D13" s="5" t="s">
         <v>23</v>
+      </c>
+      <c r="F13" s="34">
+        <v>1</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1107,7 +1134,9 @@
         <v>51</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="38">
+        <v>1</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1122,7 +1151,9 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="I15" s="38">
+        <v>1</v>
+      </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
@@ -1154,6 +1185,9 @@
       <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E18" s="34">
+        <v>0.95</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1168,38 +1202,79 @@
       <c r="D19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="E19" s="34">
+        <v>1</v>
+      </c>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38">
+        <v>1</v>
+      </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="J19" s="38">
+        <v>1</v>
+      </c>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="E20" s="34">
+        <v>1</v>
+      </c>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38">
+        <v>1</v>
+      </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="E21" s="34">
+        <v>1</v>
+      </c>
+      <c r="I21" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="35">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="34">
+        <v>1</v>
+      </c>
+      <c r="J22" s="35">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="34">
+        <v>1</v>
+      </c>
+      <c r="J23" s="35">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
@@ -1212,7 +1287,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="14">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1233,8 +1308,8 @@
       <c r="C27" t="s">
         <v>50</v>
       </c>
-      <c r="F27" s="34">
-        <v>0.5</v>
+      <c r="G27" s="34">
+        <v>0.95</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1244,22 +1319,47 @@
       <c r="C28" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="34">
+      <c r="H28" s="35">
+        <v>1</v>
+      </c>
+      <c r="I28" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <v>5</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E31" s="8">
         <v>4</v>
       </c>
-      <c r="F29" s="14">
-        <v>0</v>
+      <c r="F31" s="14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assignment 2 - Task 6 - Week 13 - Answer
1. Score Algorithm.
2. YouTube link.
</commit_message>
<xml_diff>
--- a/local snake game/Product-backlog-AH-23594256.xlsx
+++ b/local snake game/Product-backlog-AH-23594256.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Week 9</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>Test start and pause</t>
+  </si>
+  <si>
+    <t>3.2.4</t>
+  </si>
+  <si>
+    <t>3.2.5</t>
+  </si>
+  <si>
+    <t>score algorithm</t>
+  </si>
+  <si>
+    <t>Test score</t>
   </si>
 </sst>
 </file>
@@ -372,13 +384,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,7 +697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,40 +725,40 @@
       <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="36"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -904,10 +916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,10 +1112,10 @@
         <v>22</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="38">
+      <c r="H12" s="36">
         <v>0.98</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I12" s="36">
         <v>1</v>
       </c>
       <c r="J12" s="6"/>
@@ -1134,7 +1146,7 @@
         <v>51</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="38">
+      <c r="H14" s="36">
         <v>1</v>
       </c>
       <c r="I14" s="6"/>
@@ -1151,7 +1163,7 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="38">
+      <c r="I15" s="36">
         <v>1</v>
       </c>
       <c r="J15" s="6"/>
@@ -1186,7 +1198,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="34">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1205,12 +1217,12 @@
       <c r="E19" s="34">
         <v>1</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38">
+      <c r="G19" s="36"/>
+      <c r="H19" s="36">
         <v>1</v>
       </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="38">
+      <c r="J19" s="36">
         <v>1</v>
       </c>
       <c r="K19" s="6"/>
@@ -1227,9 +1239,9 @@
       <c r="E20" s="34">
         <v>1</v>
       </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38">
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36">
         <v>1</v>
       </c>
       <c r="J20" s="6"/>
@@ -1253,7 +1265,9 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>58</v>
       </c>
@@ -1265,7 +1279,9 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="D23" s="5" t="s">
         <v>59</v>
       </c>
@@ -1273,6 +1289,17 @@
         <v>1</v>
       </c>
       <c r="J23" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="34">
+        <v>1</v>
+      </c>
+      <c r="K24" s="35">
         <v>1</v>
       </c>
     </row>
@@ -1287,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="14">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1311,6 +1338,9 @@
       <c r="G27" s="34">
         <v>0.95</v>
       </c>
+      <c r="K27" s="35">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
@@ -1349,16 +1379,28 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="34"/>
+      <c r="K31" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
         <v>5</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E32" s="8">
         <v>4</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F32" s="14">
         <v>1</v>
       </c>
     </row>

</xml_diff>